<commit_message>
updated program + report
</commit_message>
<xml_diff>
--- a/AI_Assignment/depth and breadth data.xlsx
+++ b/AI_Assignment/depth and breadth data.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17830"/>
-  <workbookPr defaultThemeVersion="166925"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LENOVO\Documents\Visual Studio 2017\Projects\AI_Assignment\AI_Assignment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Justin\Documents\Git\AI_Assignment\AI_Assignment\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -29,7 +29,7 @@
     <definedName name="_xlchart.v1.8" hidden="1">Sheet1!$B$1</definedName>
     <definedName name="_xlchart.v1.9" hidden="1">Sheet1!$B$2:$B$8</definedName>
   </definedNames>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="6">
   <si>
     <t>depth - map1</t>
   </si>
@@ -52,11 +52,17 @@
   <si>
     <t>breadth - map 1</t>
   </si>
+  <si>
+    <t>Node Expansions</t>
+  </si>
+  <si>
+    <t>depth - map 1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -106,7 +112,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -151,6 +157,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -309,7 +316,7 @@
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000002-B044-43B1-9C5C-28D4E88245D3}"/>
             </c:ext>
@@ -326,11 +333,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="380531488"/>
-        <c:axId val="380531816"/>
+        <c:axId val="216268056"/>
+        <c:axId val="216271192"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="380531488"/>
+        <c:axId val="216268056"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -361,6 +368,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -425,7 +433,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380531816"/>
+        <c:crossAx val="216271192"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -433,7 +441,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="380531816"/>
+        <c:axId val="216271192"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -478,6 +486,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -536,7 +545,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380531488"/>
+        <c:crossAx val="216268056"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -597,7 +606,7 @@
 </file>
 
 <file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -642,6 +651,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -742,40 +752,42 @@
           </c:dLbls>
           <c:cat>
             <c:numRef>
-              <c:f>Sheet1!$C$2:$C$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$C$11:$C$13</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$C$11:$C$13</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>13</c:v>
+                  <c:v>37</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>15</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>17</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>27</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>29</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>35</c:v>
+                  <c:v>39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Sheet1!$B$2:$B$8</c:f>
+              <c:extLst>
+                <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                  <c15:fullRef>
+                    <c15:sqref>Sheet1!$B$2:$B$8</c15:sqref>
+                  </c15:fullRef>
+                </c:ext>
+              </c:extLst>
+              <c:f>Sheet1!$B$2:$B$4</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="3"/>
                 <c:pt idx="0">
                   <c:v>2</c:v>
                 </c:pt>
@@ -785,24 +797,12 @@
                 <c:pt idx="2">
                   <c:v>2</c:v>
                 </c:pt>
-                <c:pt idx="3">
-                  <c:v>5</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>3</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>4</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>4</c:v>
-                </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-40E2-45F9-B9B8-4442F0D47225}"/>
+              <c16:uniqueId val="{00000002-B044-43B1-9C5C-28D4E88245D3}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -817,11 +817,11 @@
         </c:dLbls>
         <c:gapWidth val="100"/>
         <c:overlap val="-24"/>
-        <c:axId val="380531488"/>
-        <c:axId val="380531816"/>
+        <c:axId val="211164560"/>
+        <c:axId val="146910768"/>
       </c:barChart>
       <c:catAx>
-        <c:axId val="380531488"/>
+        <c:axId val="211164560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -847,11 +847,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="en-AU"/>
-                  <a:t>Path Count</a:t>
+                  <a:t>Node Expansions</a:t>
                 </a:r>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -916,7 +917,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380531816"/>
+        <c:crossAx val="146910768"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -924,7 +925,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="380531816"/>
+        <c:axId val="146910768"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -969,6 +970,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1027,7 +1029,556 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="380531488"/>
+        <c:crossAx val="211164560"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:gradFill flip="none" rotWithShape="1">
+      <a:gsLst>
+        <a:gs pos="0">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:gs>
+        <a:gs pos="100000">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="85000"/>
+            <a:lumOff val="15000"/>
+          </a:schemeClr>
+        </a:gs>
+      </a:gsLst>
+      <a:path path="circle">
+        <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+      </a:path>
+      <a:tileRect/>
+    </a:gradFill>
+    <a:ln>
+      <a:noFill/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="95000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:effectLst>
+                  <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                    <a:prstClr val="black">
+                      <a:alpha val="40000"/>
+                    </a:prstClr>
+                  </a:outerShdw>
+                </a:effectLst>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>Map 1 DFS</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:layout/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1600" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="100" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:effectLst>
+                <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+                  <a:prstClr val="black">
+                    <a:alpha val="40000"/>
+                  </a:prstClr>
+                </a:outerShdw>
+              </a:effectLst>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Sheet1!$B$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Iterations</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:gradFill rotWithShape="1">
+              <a:gsLst>
+                <a:gs pos="0">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="103000"/>
+                    <a:lumMod val="102000"/>
+                    <a:tint val="94000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="50000">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="110000"/>
+                    <a:lumMod val="100000"/>
+                    <a:shade val="100000"/>
+                  </a:schemeClr>
+                </a:gs>
+                <a:gs pos="100000">
+                  <a:schemeClr val="accent1">
+                    <a:lumMod val="99000"/>
+                    <a:satMod val="120000"/>
+                    <a:shade val="78000"/>
+                  </a:schemeClr>
+                </a:gs>
+              </a:gsLst>
+              <a:lin ang="5400000" scaled="0"/>
+            </a:gradFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst>
+              <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+                <a:srgbClr val="000000">
+                  <a:alpha val="63000"/>
+                </a:srgbClr>
+              </a:outerShdw>
+            </a:effectLst>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:dLbls>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" lIns="38100" tIns="19050" rIns="38100" bIns="19050" anchor="ctr" anchorCtr="1">
+                <a:spAutoFit/>
+              </a:bodyPr>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:txPr>
+            <c:dLblPos val="inEnd"/>
+            <c:showLegendKey val="0"/>
+            <c:showVal val="1"/>
+            <c:showCatName val="0"/>
+            <c:showSerName val="0"/>
+            <c:showPercent val="0"/>
+            <c:showBubbleSize val="0"/>
+            <c:showLeaderLines val="0"/>
+            <c:extLst>
+              <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{CE6537A1-D6FC-4f65-9D91-7224C49458BB}">
+                <c15:layout/>
+                <c15:showLeaderLines val="1"/>
+                <c15:leaderLines>
+                  <c:spPr>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="lt1">
+                          <a:lumMod val="95000"/>
+                          <a:alpha val="54000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c15:leaderLines>
+              </c:ext>
+            </c:extLst>
+          </c:dLbls>
+          <c:cat>
+            <c:numRef>
+              <c:f>Sheet1!$C$23:$C$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>32</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>39</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Sheet1!$B$23:$B$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+        </c:ser>
+        <c:dLbls>
+          <c:dLblPos val="inEnd"/>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="1"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="100"/>
+        <c:overlap val="-24"/>
+        <c:axId val="320885656"/>
+        <c:axId val="320882912"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="320885656"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Node Expansions</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="95000"/>
+                <a:alpha val="54000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="320882912"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="320882912"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="95000"/>
+                  <a:alpha val="10000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="lt1">
+                        <a:lumMod val="85000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-AU"/>
+                  <a:t>Iterations</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="all" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="lt1">
+                      <a:lumMod val="85000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="85000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="320885656"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1167,6 +1718,46 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
@@ -1664,6 +2255,502 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" b="1" kern="1200" cap="all"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:gradFill flip="none" rotWithShape="1">
+        <a:gsLst>
+          <a:gs pos="0">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="65000"/>
+              <a:lumOff val="35000"/>
+            </a:schemeClr>
+          </a:gs>
+          <a:gs pos="100000">
+            <a:schemeClr val="dk1">
+              <a:lumMod val="85000"/>
+              <a:lumOff val="15000"/>
+            </a:schemeClr>
+          </a:gs>
+        </a:gsLst>
+        <a:path path="circle">
+          <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+        </a:path>
+        <a:tileRect/>
+      </a:gradFill>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="34925" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="6"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="3"/>
+    <cs:effectRef idx="3"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="10000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="5000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:prstDash val="dash"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="95000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1600" b="1" kern="1200" spc="100" baseline="0">
+      <a:effectLst>
+        <a:outerShdw blurRad="50800" dist="38100" dir="5400000" algn="t" rotWithShape="0">
+          <a:prstClr val="black">
+            <a:alpha val="40000"/>
+          </a:prstClr>
+        </a:outerShdw>
+      </a:effectLst>
+    </cs:defRPr>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="95000"/>
+            <a:alpha val="54000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="209">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2179,7 +3266,7 @@
         <xdr:cNvPr id="5" name="Chart 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{D5BA8CA1-5ABB-4490-A71E-3C97B4454EFC}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5BA8CA1-5ABB-4490-A71E-3C97B4454EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2200,22 +3287,22 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>16</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>552450</xdr:colOff>
+      <xdr:row>17</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>447675</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>247650</xdr:colOff>
       <xdr:row>31</xdr:row>
-      <xdr:rowOff>19050</xdr:rowOff>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="6" name="Chart 5">
+        <xdr:cNvPr id="4" name="Chart 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{5DBF841D-C0F3-459D-96CF-1C6F867EF0CB}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5BA8CA1-5ABB-4490-A71E-3C97B4454EFC}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2230,6 +3317,44 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>190500</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>495300</xdr:colOff>
+      <xdr:row>48</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="7" name="Chart 6">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{D5BA8CA1-5ABB-4490-A71E-3C97B4454EFC}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -2535,17 +3660,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="O45" sqref="O45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="15.42578125" customWidth="1"/>
     <col min="2" max="2" width="10" customWidth="1"/>
-    <col min="3" max="3" width="11" customWidth="1"/>
+    <col min="3" max="3" width="23.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -2623,7 +3748,106 @@
         <v>2</v>
       </c>
       <c r="C10" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B11">
+        <v>8</v>
+      </c>
+      <c r="C11">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B12">
+        <v>4</v>
+      </c>
+      <c r="C12">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B13">
+        <v>12</v>
+      </c>
+      <c r="C13">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" t="s">
+        <v>5</v>
+      </c>
+      <c r="B22" t="s">
+        <v>2</v>
+      </c>
+      <c r="C22" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B23">
+        <v>2</v>
+      </c>
+      <c r="C23">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B24">
+        <v>2</v>
+      </c>
+      <c r="C24">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B25">
+        <v>4</v>
+      </c>
+      <c r="C25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B26">
+        <v>2</v>
+      </c>
+      <c r="C26">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B27">
         <v>1</v>
+      </c>
+      <c r="C27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B28">
+        <v>3</v>
+      </c>
+      <c r="C28">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B29">
+        <v>2</v>
+      </c>
+      <c r="C29">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="B30">
+        <v>8</v>
+      </c>
+      <c r="C30">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>